<commit_message>
Add more products $MSFT
</commit_message>
<xml_diff>
--- a/$MSFT.xlsx
+++ b/$MSFT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189690F7-E2F9-4CD9-95CA-52E0B1C38622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0698C55-6C79-4008-B7D1-C2D7BB077A9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{576A60CD-F651-4890-A3F2-1DFF46C64604}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{576A60CD-F651-4890-A3F2-1DFF46C64604}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>$MSFT</t>
   </si>
@@ -257,6 +257,42 @@
   </si>
   <si>
     <t>FY33</t>
+  </si>
+  <si>
+    <t>Software Development</t>
+  </si>
+  <si>
+    <t>Visual Studio</t>
+  </si>
+  <si>
+    <t>VS Code</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Github CoPilot</t>
+  </si>
+  <si>
+    <t>.NET</t>
+  </si>
+  <si>
+    <t>TypeScript</t>
+  </si>
+  <si>
+    <t>OneDrive</t>
+  </si>
+  <si>
+    <t>Azure Machine Learning</t>
+  </si>
+  <si>
+    <t>Hololens (mixed reality AR headset)</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
   </si>
 </sst>
 </file>
@@ -473,18 +509,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -496,19 +520,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -560,6 +572,30 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -941,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FC4347-A5C6-409A-A3AE-A54C952422EE}">
-  <dimension ref="B2:Y40"/>
+  <dimension ref="B2:Z40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -952,793 +988,842 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="G5" s="6" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="G5" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="8"/>
-      <c r="U5" s="9" t="s">
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="42"/>
+      <c r="U5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V5" s="39"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4">
         <v>256.88</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="G6" s="31">
+      <c r="D6" s="16"/>
+      <c r="G6" s="23">
         <v>44958</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
-      <c r="U6" s="10" t="s">
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="25"/>
+      <c r="U6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="12">
         <v>7440</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="33"/>
-      <c r="U7" s="12" t="s">
+      <c r="D7" s="16"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="25"/>
+      <c r="U7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="12">
         <f>C6*C7</f>
         <v>1911187.2</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="G8" s="31">
+      <c r="D8" s="16"/>
+      <c r="G8" s="23">
         <v>44927</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="33"/>
-      <c r="U8" s="12" t="s">
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="25"/>
+      <c r="U8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="24"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="34" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="16"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="33"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="25"/>
+      <c r="U9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="24"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="33"/>
-      <c r="U10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C10" s="12"/>
+      <c r="D10" s="16"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="25"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="12">
         <f>C9-C10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="33"/>
-      <c r="U11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D11" s="16"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="25"/>
+      <c r="U11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="13">
         <f>C8-C11</f>
         <v>1911187.2</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="G12" s="31">
+      <c r="D12" s="17"/>
+      <c r="G12" s="23">
         <v>44927</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="33"/>
-      <c r="U12" s="12" t="s">
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="25"/>
+      <c r="U12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G13" s="14"/>
+      <c r="H13" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="25"/>
+      <c r="U13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G13" s="22"/>
-      <c r="H13" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="33"/>
-      <c r="U13" s="12" t="s">
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G14" s="14"/>
+      <c r="H14" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="25"/>
+      <c r="U14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G14" s="22"/>
-      <c r="H14" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="33"/>
-      <c r="U14" s="12" t="s">
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B15" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="25"/>
+      <c r="U15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="33"/>
-      <c r="U15" s="12" t="s">
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="38"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="25"/>
+      <c r="U16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B16" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="33"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-    </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="14" t="s">
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="33"/>
-      <c r="U17" s="10" t="s">
+      <c r="D17" s="38"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="25"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="25"/>
+      <c r="U18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-    </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="33"/>
-      <c r="U18" s="12" t="s">
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="25"/>
+      <c r="U19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-    </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="33"/>
-      <c r="U19" s="13" t="s">
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G20" s="14"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="25"/>
+      <c r="U20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-    </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G20" s="22"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="33"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-    </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G21" s="22"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="33"/>
-      <c r="U21" s="10" t="s">
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G21" s="14"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="25"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B22" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="25"/>
+      <c r="U22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-    </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="33"/>
-      <c r="U22" s="12" t="s">
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="25"/>
+      <c r="U23" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-    </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B23" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="16"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="33"/>
-      <c r="U23" s="38" t="s">
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+    </row>
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="37">
+        <v>1975</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="25"/>
+      <c r="U24" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-    </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B24" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="15">
-        <v>1975</v>
-      </c>
-      <c r="D24" s="16"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="33"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-    </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B25" s="22" t="s">
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+    </row>
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="37">
         <v>1986</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="33"/>
-      <c r="U25" s="10" t="s">
+      <c r="D25" s="38"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="25"/>
+      <c r="U25" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+    </row>
+    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B26" s="14"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="25"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+    </row>
+    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B27" s="14"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="25"/>
+      <c r="U27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-    </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B26" s="22"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="33"/>
-      <c r="U26" s="12" t="s">
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+    </row>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B28" s="14"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="25"/>
+      <c r="U28" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-    </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B27" s="22"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="32"/>
-      <c r="Q27" s="32"/>
-      <c r="R27" s="33"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-    </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B28" s="22"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="32"/>
-      <c r="R28" s="33"/>
-      <c r="U28" s="10" t="s">
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+    </row>
+    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B29" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="25"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+    </row>
+    <row r="30" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="36"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="25"/>
+      <c r="U30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-    </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B29" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="33"/>
-      <c r="U29" s="39" t="s">
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+    </row>
+    <row r="31" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G31" s="14"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="25"/>
+      <c r="U31" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-    </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="19"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="32"/>
-      <c r="R30" s="33"/>
-      <c r="U30" s="12" t="s">
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+    </row>
+    <row r="32" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G32" s="14"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="25"/>
+      <c r="U32" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+    </row>
+    <row r="33" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="G33" s="15"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="29"/>
+      <c r="U33" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-    </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G31" s="22"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="32"/>
-      <c r="R31" s="33"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
-    </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="G32" s="22"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="33"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-    </row>
-    <row r="33" spans="7:25" x14ac:dyDescent="0.2">
-      <c r="G33" s="23"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="37"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-    </row>
-    <row r="36" spans="7:25" x14ac:dyDescent="0.2">
-      <c r="G36" s="26" t="s">
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+    </row>
+    <row r="34" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="U34" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="G36" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="7:25" x14ac:dyDescent="0.2">
-      <c r="G37" s="27" t="s">
+    <row r="37" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="G37" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="7:25" x14ac:dyDescent="0.2">
-      <c r="G38" s="30" t="s">
+    <row r="38" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="G38" s="22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="7:25" x14ac:dyDescent="0.2">
-      <c r="G39" s="30" t="s">
+    <row r="39" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="G39" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="7:25" x14ac:dyDescent="0.2">
-      <c r="G40" s="30"/>
+    <row r="40" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="G40" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="U5:Y5"/>
     <mergeCell ref="G5:R5"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
@@ -1747,9 +1832,16 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="U5:Z5"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="U29" r:id="rId1" xr:uid="{77D798DA-BEC3-4A4F-B569-E742FCC67D61}"/>
+    <hyperlink ref="U31" r:id="rId1" xr:uid="{77D798DA-BEC3-4A4F-B569-E742FCC67D61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
@@ -1761,11 +1853,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA9C7E-0554-4827-A039-42D80E639FDF}">
   <dimension ref="B1:AP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B2:B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1774,70 +1866,70 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="X1" s="40" t="s">
+    <row r="1" spans="2:42" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="40" t="s">
+      <c r="Y1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="40" t="s">
+      <c r="Z1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="AA1" s="40" t="s">
+      <c r="AA1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="AB1" s="40" t="s">
+      <c r="AB1" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" s="40" t="s">
+      <c r="AC1" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="AD1" s="40" t="s">
+      <c r="AD1" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="40" t="s">
+      <c r="AE1" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="AF1" s="40" t="s">
+      <c r="AF1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="40" t="s">
+      <c r="AG1" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="40" t="s">
+      <c r="AH1" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AI1" s="40" t="s">
+      <c r="AI1" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="AJ1" s="40" t="s">
+      <c r="AJ1" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="40" t="s">
+      <c r="AK1" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="AL1" s="40" t="s">
+      <c r="AL1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="AM1" s="40" t="s">
+      <c r="AM1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="AN1" s="40" t="s">
+      <c r="AN1" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="AO1" s="40" t="s">
+      <c r="AO1" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="AP1" s="40" t="s">
+      <c r="AP1" s="32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="2:42" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="41"/>
-    </row>
-    <row r="3" spans="2:42" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="41"/>
+    <row r="2" spans="2:42" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="33"/>
+    </row>
+    <row r="3" spans="2:42" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
$MSFT OpenAI preview event notes
</commit_message>
<xml_diff>
--- a/$MSFT.xlsx
+++ b/$MSFT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0698C55-6C79-4008-B7D1-C2D7BB077A9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F845542-9152-4978-8B3C-987E078F2D7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{576A60CD-F651-4890-A3F2-1DFF46C64604}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>$MSFT</t>
   </si>
@@ -293,13 +293,49 @@
   </si>
   <si>
     <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Preview of Bing with ChatGT integration</t>
+  </si>
+  <si>
+    <t>Search results show with new right hand tab with GPT enhanced results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Search" and "Chat" are also entirely separate tabs if you want traditional search or new chatbot </t>
+  </si>
+  <si>
+    <t>Chat is basically ChatGPT with suggested prompt replies to speed up input</t>
+  </si>
+  <si>
+    <t>MSFT host press event to preview Bing-GPT integration, showing new search &amp; chat layout and features</t>
+  </si>
+  <si>
+    <t>Second preview is of GPT integration into the Edge browser</t>
+  </si>
+  <si>
+    <t>Shows split-screen feature where GPT can use browser content to generate information from prompts</t>
+  </si>
+  <si>
+    <t>Analysing/summarising/comparing earnings rpeorts for Gap &amp; LULU and returning them in a table</t>
+  </si>
+  <si>
+    <t>Stackoverflow example</t>
+  </si>
+  <si>
+    <t>Creating content for LinkedIn</t>
+  </si>
+  <si>
+    <t>Feb 2023 OpenAI Integration Preview Event</t>
+  </si>
+  <si>
+    <t>Preview OpenAI integration into Bing.com is released for wide-spread usage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +415,18 @@
       <b/>
       <sz val="8"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.14999847407452621"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -502,21 +550,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,40 +601,62 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -977,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FC4347-A5C6-409A-A3AE-A54C952422EE}">
-  <dimension ref="B2:Z40"/>
+  <dimension ref="B2:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37:R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1018,14 +1080,14 @@
       <c r="P5" s="41"/>
       <c r="Q5" s="41"/>
       <c r="R5" s="42"/>
-      <c r="U5" s="39" t="s">
+      <c r="U5" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="42"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1034,274 +1096,272 @@
       <c r="C6" s="4">
         <v>256.88</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="G6" s="23">
-        <v>44958</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="25"/>
-      <c r="U6" s="6" t="s">
+      <c r="D6" s="12"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="21"/>
+      <c r="U6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="6" t="s">
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="21"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="8">
         <v>7440</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="25"/>
-      <c r="U7" s="8" t="s">
+      <c r="D7" s="12"/>
+      <c r="G7" s="19">
+        <v>44958</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="21"/>
+      <c r="U7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="8" t="s">
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="21"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="8">
         <f>C6*C7</f>
         <v>1911187.2</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="G8" s="23">
-        <v>44927</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="25"/>
-      <c r="U8" s="8" t="s">
+      <c r="D8" s="12"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="21"/>
+      <c r="U8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="8" t="s">
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="21"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="16"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="25"/>
-      <c r="U9" s="8" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="12"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="21"/>
+      <c r="U9" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="8" t="s">
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="21"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="16"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="25"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="8" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="12"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="21"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="8">
         <f>C9-C10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="25"/>
-      <c r="U11" s="6" t="s">
+      <c r="D11" s="12"/>
+      <c r="G11" s="19">
+        <v>44958</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="21"/>
+      <c r="U11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="8" t="s">
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="21"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="9">
         <f>C8-C11</f>
         <v>1911187.2</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="G12" s="23">
+      <c r="D12" s="13"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="21"/>
+      <c r="U12" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="21"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="G13" s="19">
         <v>44927</v>
       </c>
-      <c r="H12" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="25"/>
-      <c r="U12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="G13" s="14"/>
-      <c r="H13" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="25"/>
-      <c r="U13" s="8" t="s">
+      <c r="H13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="21"/>
+      <c r="U13" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="21"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="G14" s="14"/>
-      <c r="H14" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="25"/>
-      <c r="U14" s="8" t="s">
+      <c r="G14" s="10"/>
+      <c r="H14" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
+      <c r="U14" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="6" t="s">
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="21"/>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B15" s="40" t="s">
@@ -1309,182 +1369,190 @@
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="42"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="25"/>
-      <c r="U15" s="8" t="s">
+      <c r="G15" s="10"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="21"/>
+      <c r="U15" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="8" t="s">
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="21"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="25"/>
-      <c r="U16" s="8" t="s">
+      <c r="D16" s="44"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="21"/>
+      <c r="U16" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="21"/>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="25"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
+      <c r="D17" s="44"/>
+      <c r="G17" s="19">
+        <v>44927</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="21"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="21"/>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="25"/>
-      <c r="U18" s="6" t="s">
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="21"/>
+      <c r="U18" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="21"/>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="25"/>
-      <c r="U19" s="8" t="s">
+      <c r="D19" s="39"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="21"/>
+      <c r="U19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="21"/>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="G20" s="14"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="25"/>
-      <c r="U20" s="9" t="s">
+      <c r="G20" s="10"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="21"/>
+      <c r="U20" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="21"/>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="G21" s="14"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="25"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="21"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="21"/>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B22" s="40" t="s">
@@ -1492,337 +1560,392 @@
       </c>
       <c r="C22" s="41"/>
       <c r="D22" s="42"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="25"/>
-      <c r="U22" s="6" t="s">
+      <c r="G22" s="10"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="21"/>
+      <c r="U22" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="21"/>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="38"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="25"/>
-      <c r="U23" s="8" t="s">
+      <c r="D23" s="44"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="21"/>
+      <c r="U23" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="21"/>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="43">
         <v>1975</v>
       </c>
-      <c r="D24" s="38"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="25"/>
-      <c r="U24" s="30" t="s">
+      <c r="D24" s="44"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="21"/>
+      <c r="U24" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="21"/>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="43">
         <v>1986</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="25"/>
-      <c r="U25" s="8" t="s">
+      <c r="D25" s="44"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="21"/>
+      <c r="U25" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="V25" s="7"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="7"/>
-      <c r="Y25" s="7"/>
-      <c r="Z25" s="7"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="21"/>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B26" s="14"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="25"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="7"/>
-      <c r="Y26" s="7"/>
-      <c r="Z26" s="7"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="21"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
+      <c r="Z26" s="21"/>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B27" s="14"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="38"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="25"/>
-      <c r="U27" s="6" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="21"/>
+      <c r="U27" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="21"/>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B28" s="14"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="25"/>
-      <c r="U28" s="8" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="21"/>
+      <c r="U28" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="V28" s="7"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-      <c r="Z28" s="7"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="21"/>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="25"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="21"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20"/>
+      <c r="Z29" s="21"/>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="25"/>
-      <c r="U30" s="6" t="s">
+      <c r="D30" s="39"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="21"/>
+      <c r="U30" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="V30" s="7"/>
-      <c r="W30" s="7"/>
-      <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="20"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="21"/>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="G31" s="14"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="25"/>
-      <c r="U31" s="31" t="s">
+      <c r="G31" s="10"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="21"/>
+      <c r="U31" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="21"/>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="G32" s="14"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="25"/>
-      <c r="U32" s="8" t="s">
+      <c r="G32" s="10"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="21"/>
+      <c r="U32" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="21"/>
     </row>
     <row r="33" spans="7:26" x14ac:dyDescent="0.2">
-      <c r="G33" s="15"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="28"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="29"/>
-      <c r="U33" s="8" t="s">
+      <c r="G33" s="11"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="25"/>
+      <c r="U33" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="21"/>
     </row>
     <row r="34" spans="7:26" x14ac:dyDescent="0.2">
-      <c r="U34" s="8" t="s">
+      <c r="U34" s="35" t="s">
         <v>85</v>
       </c>
+      <c r="V34" s="36"/>
+      <c r="W34" s="36"/>
+      <c r="X34" s="36"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="37"/>
     </row>
     <row r="36" spans="7:26" x14ac:dyDescent="0.2">
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="14" t="s">
         <v>47</v>
       </c>
+      <c r="Q36" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="37" spans="7:26" x14ac:dyDescent="0.2">
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="15" t="s">
         <v>48</v>
       </c>
+      <c r="Q37" s="46" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="38" spans="7:26" x14ac:dyDescent="0.2">
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="18" t="s">
         <v>53</v>
       </c>
+      <c r="Q38" s="46" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="39" spans="7:26" x14ac:dyDescent="0.2">
-      <c r="G39" s="22" t="s">
+      <c r="G39" s="18" t="s">
         <v>54</v>
       </c>
+      <c r="Q39" s="46" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="40" spans="7:26" x14ac:dyDescent="0.2">
-      <c r="G40" s="22"/>
+      <c r="G40" s="18"/>
+      <c r="Q40" s="47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="Q41" s="45"/>
+    </row>
+    <row r="42" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="Q42" s="46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="Q43" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="Q44" s="47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="Q45" s="47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="7:26" x14ac:dyDescent="0.2">
+      <c r="Q46" s="48" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="U5:Z5"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="G5:R5"/>
     <mergeCell ref="B22:D22"/>
@@ -1832,13 +1955,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="U5:Z5"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="U31" r:id="rId1" xr:uid="{77D798DA-BEC3-4A4F-B569-E742FCC67D61}"/>
@@ -1866,70 +1982,70 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="X1" s="32" t="s">
+    <row r="1" spans="2:42" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="32" t="s">
+      <c r="Y1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="AA1" s="32" t="s">
+      <c r="AA1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="AB1" s="32" t="s">
+      <c r="AB1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" s="32" t="s">
+      <c r="AC1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="AD1" s="32" t="s">
+      <c r="AD1" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="32" t="s">
+      <c r="AE1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="AF1" s="32" t="s">
+      <c r="AF1" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="32" t="s">
+      <c r="AG1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="32" t="s">
+      <c r="AH1" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="AI1" s="32" t="s">
+      <c r="AI1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AJ1" s="32" t="s">
+      <c r="AJ1" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="32" t="s">
+      <c r="AK1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="AL1" s="32" t="s">
+      <c r="AL1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="AM1" s="32" t="s">
+      <c r="AM1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="AN1" s="32" t="s">
+      <c r="AN1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="AO1" s="32" t="s">
+      <c r="AO1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="AP1" s="32" t="s">
+      <c r="AP1" s="26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="2:42" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="33"/>
-    </row>
-    <row r="3" spans="2:42" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="33"/>
+    <row r="2" spans="2:42" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="27"/>
+    </row>
+    <row r="3" spans="2:42" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>